<commit_message>
last but not least
</commit_message>
<xml_diff>
--- a/blanded_learning/src/assets/DataCSV/Filieres.xlsx
+++ b/blanded_learning/src/assets/DataCSV/Filieres.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ouss_ama\Desktop\ProjetBlendedLearning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ouss_ama\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99187FD6-53B7-4602-A199-44DA0E65CA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE4D640-B8FE-4930-A90E-E6FFECC97FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>libelle</t>
   </si>
@@ -45,21 +45,9 @@
     <t>Departement2</t>
   </si>
   <si>
-    <t>2ITE</t>
-  </si>
-  <si>
-    <t>ISIC</t>
-  </si>
-  <si>
     <t>GEE</t>
   </si>
   <si>
-    <t>Dahbi</t>
-  </si>
-  <si>
-    <t>Baidada</t>
-  </si>
-  <si>
     <t>Belhora</t>
   </si>
   <si>
@@ -79,6 +67,12 @@
   </si>
   <si>
     <t>CCC</t>
+  </si>
+  <si>
+    <t>GSP</t>
+  </si>
+  <si>
+    <t>CRRR</t>
   </si>
 </sst>
 </file>
@@ -416,10 +410,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -448,35 +442,35 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -496,7 +490,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -510,20 +504,6 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>